<commit_message>
Updated reconstruction tools with revision data
</commit_message>
<xml_diff>
--- a/reconstruction-tools-assessment/supplementary material/S10_table.xlsx
+++ b/reconstruction-tools-assessment/supplementary material/S10_table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Research_Projects\Review_reconstruction\manuscript\supplementary material\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086CBC10-3E23-40CB-9959-4EDC93AEF030}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9402"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S10 Table" sheetId="1" r:id="rId1"/>
@@ -160,9 +161,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -201,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -209,9 +210,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,11 +525,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+      <selection activeCell="C5" sqref="C5:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -587,580 +587,580 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>57.06666666666667</v>
+      <c r="B5" s="4">
+        <v>62</v>
       </c>
       <c r="C5" s="3">
-        <v>60.186418109187748</v>
+        <v>65.113182423435418</v>
       </c>
       <c r="D5" s="3">
-        <v>61.651131824234355</v>
+        <v>66.577896138482018</v>
       </c>
       <c r="E5" s="3">
-        <v>60.186418109187748</v>
+        <v>65.113182423435418</v>
       </c>
       <c r="F5" s="3">
-        <v>61.651131824234355</v>
+        <v>66.577896138482018</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>57.866666666666667</v>
+      <c r="B6" s="4">
+        <v>62.8</v>
       </c>
       <c r="C6" s="3">
-        <v>61.251664447403463</v>
+        <v>66.178428761651134</v>
       </c>
       <c r="D6" s="3">
-        <v>62.316910785619172</v>
+        <v>67.243675099866849</v>
       </c>
       <c r="E6" s="3">
-        <v>61.251664447403463</v>
+        <v>66.178428761651134</v>
       </c>
       <c r="F6" s="3">
-        <v>62.316910785619172</v>
+        <v>67.243675099866849</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>47.6</v>
+      <c r="B7" s="4">
+        <v>45.866666666666667</v>
       </c>
       <c r="C7" s="3">
-        <v>48.868175765645809</v>
+        <v>45.80559254327563</v>
       </c>
       <c r="D7" s="3">
-        <v>48.868175765645809</v>
+        <v>45.80559254327563</v>
       </c>
       <c r="E7" s="3">
-        <v>48.868175765645809</v>
+        <v>45.80559254327563</v>
       </c>
       <c r="F7" s="3">
-        <v>48.868175765645809</v>
+        <v>45.80559254327563</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>55.2</v>
+      <c r="B8" s="4">
+        <v>52.533333333333331</v>
       </c>
       <c r="C8" s="3">
-        <v>55.65912117177097</v>
+        <v>52.996005326231689</v>
       </c>
       <c r="D8" s="3">
-        <v>56.99067909454061</v>
+        <v>54.327563249001329</v>
       </c>
       <c r="E8" s="3">
-        <v>55.65912117177097</v>
+        <v>52.996005326231689</v>
       </c>
       <c r="F8" s="3">
-        <v>56.99067909454061</v>
+        <v>54.327563249001329</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>53.466666666666669</v>
+      <c r="B9" s="4">
+        <v>52</v>
       </c>
       <c r="C9" s="3">
+        <v>53.129161118508655</v>
+      </c>
+      <c r="D9" s="3">
         <v>54.593874833555262</v>
       </c>
-      <c r="D9" s="3">
-        <v>56.058588548601861</v>
-      </c>
       <c r="E9" s="3">
+        <v>53.129161118508655</v>
+      </c>
+      <c r="F9" s="3">
         <v>54.593874833555262</v>
-      </c>
-      <c r="F9" s="3">
-        <v>56.058588548601861</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>60.533333333333331</v>
+      <c r="B10" s="4">
+        <v>49.866666666666667</v>
       </c>
       <c r="C10" s="3">
-        <v>62.183754993342212</v>
+        <v>49.800266311584551</v>
       </c>
       <c r="D10" s="3">
-        <v>65.645805592543269</v>
+        <v>49.800266311584551</v>
       </c>
       <c r="E10" s="3">
-        <v>62.183754993342212</v>
+        <v>49.800266311584551</v>
       </c>
       <c r="F10" s="3">
-        <v>65.645805592543269</v>
+        <v>49.800266311584551</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
-        <v>47.866666666666667</v>
+      <c r="B11" s="4">
+        <v>62.133333333333333</v>
       </c>
       <c r="C11" s="3">
-        <v>49.134487350199734</v>
+        <v>62.583222370173104</v>
       </c>
       <c r="D11" s="3">
-        <v>49.134487350199734</v>
+        <v>66.045272969374167</v>
       </c>
       <c r="E11" s="3">
-        <v>49.134487350199734</v>
+        <v>62.583222370173104</v>
       </c>
       <c r="F11" s="3">
-        <v>49.134487350199734</v>
+        <v>66.045272969374167</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>61.466666666666669</v>
+      <c r="B12" s="4">
+        <v>62.133333333333333</v>
       </c>
       <c r="C12" s="3">
-        <v>66.3115845539281</v>
+        <v>66.577896138482018</v>
       </c>
       <c r="D12" s="3">
-        <v>71.504660452729695</v>
+        <v>71.770972037283627</v>
       </c>
       <c r="E12" s="3">
-        <v>66.3115845539281</v>
+        <v>66.577896138482018</v>
       </c>
       <c r="F12" s="3">
-        <v>71.504660452729695</v>
+        <v>71.770972037283627</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>30</v>
+      <c r="B13" s="4">
+        <v>30.8</v>
       </c>
       <c r="C13" s="3">
-        <v>31.824234354194406</v>
+        <v>33.022636484687084</v>
       </c>
       <c r="D13" s="3">
-        <v>33.688415446071907</v>
+        <v>34.886817576564582</v>
       </c>
       <c r="E13" s="3">
-        <v>33.15579227696405</v>
+        <v>35.552596537949398</v>
       </c>
       <c r="F13" s="3">
-        <v>37.816245006657788</v>
+        <v>40.213049267643143</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>30.933333333333334</v>
+      <c r="B14" s="4">
+        <v>32.133333333333333</v>
       </c>
       <c r="C14" s="3">
-        <v>33.022636484687084</v>
+        <v>34.221038615179758</v>
       </c>
       <c r="D14" s="3">
-        <v>34.886817576564582</v>
+        <v>36.085219707057256</v>
       </c>
       <c r="E14" s="3">
-        <v>34.354194407456724</v>
+        <v>36.75099866844208</v>
       </c>
       <c r="F14" s="3">
-        <v>39.014647137150469</v>
+        <v>41.411451398135817</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>28.133333333333333</v>
+      <c r="B15" s="4">
+        <v>29.066666666666666</v>
       </c>
       <c r="C15" s="3">
-        <v>29.427430093209054</v>
+        <v>30.359520639147803</v>
       </c>
       <c r="D15" s="3">
-        <v>31.291611185086552</v>
+        <v>32.223701731025301</v>
       </c>
       <c r="E15" s="3">
-        <v>30.758988015978694</v>
+        <v>31.824234354194406</v>
       </c>
       <c r="F15" s="3">
-        <v>35.419440745672439</v>
+        <v>36.484687083888147</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>27.466666666666665</v>
+      <c r="B16" s="4">
+        <v>28.4</v>
       </c>
       <c r="C16" s="3">
-        <v>28.761651131824234</v>
+        <v>29.693741677762983</v>
       </c>
       <c r="D16" s="3">
-        <v>30.492676431424766</v>
+        <v>31.424766977363515</v>
       </c>
       <c r="E16" s="3">
-        <v>30.093209054593874</v>
+        <v>31.158455392809586</v>
       </c>
       <c r="F16" s="3">
-        <v>34.48735019973369</v>
+        <v>35.552596537949398</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
-        <v>30</v>
+      <c r="B17" s="4">
+        <v>30.8</v>
       </c>
       <c r="C17" s="3">
-        <v>31.824234354194406</v>
+        <v>33.022636484687084</v>
       </c>
       <c r="D17" s="3">
-        <v>33.688415446071907</v>
+        <v>34.886817576564582</v>
       </c>
       <c r="E17" s="3">
-        <v>33.15579227696405</v>
+        <v>35.552596537949398</v>
       </c>
       <c r="F17" s="3">
-        <v>37.816245006657788</v>
+        <v>40.213049267643143</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3">
-        <v>36.666666666666664</v>
+      <c r="B18" s="4">
+        <v>38.533333333333331</v>
       </c>
       <c r="C18" s="3">
-        <v>41.145139813581892</v>
+        <v>41.944074567243675</v>
       </c>
       <c r="D18" s="3">
-        <v>49.001331557922768</v>
+        <v>50.599201065246341</v>
       </c>
       <c r="E18" s="3">
-        <v>44.074567243675098</v>
+        <v>44.873501997336881</v>
       </c>
       <c r="F18" s="3">
-        <v>52.330226364846872</v>
+        <v>55.126498002663119</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
-        <v>35.733333333333334</v>
+      <c r="B19" s="4">
+        <v>37.6</v>
       </c>
       <c r="C19" s="3">
-        <v>39.813581890812252</v>
+        <v>40.612516644474034</v>
       </c>
       <c r="D19" s="3">
-        <v>47.536617842876169</v>
+        <v>49.134487350199734</v>
       </c>
       <c r="E19" s="3">
-        <v>42.743009320905458</v>
+        <v>43.54194407456724</v>
       </c>
       <c r="F19" s="3">
-        <v>50.865512649800266</v>
+        <v>53.661784287616513</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3">
-        <v>30.933333333333334</v>
+      <c r="B20" s="4">
+        <v>33.466666666666669</v>
       </c>
       <c r="C20" s="3">
-        <v>20.639147802929429</v>
+        <v>22.63648468708389</v>
       </c>
       <c r="D20" s="3">
-        <v>35.552596537949398</v>
+        <v>37.949400798934754</v>
       </c>
       <c r="E20" s="3">
-        <v>22.103861517976032</v>
+        <v>24.900133155792275</v>
       </c>
       <c r="F20" s="3">
-        <v>39.41411451398136</v>
+        <v>43.408788282290281</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3">
-        <v>31.333333333333332</v>
+      <c r="B21" s="4">
+        <v>34</v>
       </c>
       <c r="C21" s="3">
-        <v>20.905459387483354</v>
+        <v>22.902796271637815</v>
       </c>
       <c r="D21" s="3">
-        <v>36.085219707057256</v>
+        <v>38.482023968042611</v>
       </c>
       <c r="E21" s="3">
-        <v>22.370173102529961</v>
+        <v>25.166444740346204</v>
       </c>
       <c r="F21" s="3">
-        <v>39.946737683089218</v>
+        <v>43.941411451398139</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
-        <v>30.666666666666668</v>
+      <c r="B22" s="4">
+        <v>33.466666666666669</v>
       </c>
       <c r="C22" s="3">
-        <v>20.639147802929429</v>
+        <v>22.769640479360852</v>
       </c>
       <c r="D22" s="3">
-        <v>35.552596537949398</v>
+        <v>38.08255659121172</v>
       </c>
       <c r="E22" s="3">
-        <v>22.237017310252995</v>
+        <v>25.033288948069242</v>
       </c>
       <c r="F22" s="3">
-        <v>39.547270306258319</v>
+        <v>43.54194407456724</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <v>33.6</v>
+      <c r="B23" s="4">
+        <v>36.4</v>
       </c>
       <c r="C23" s="3">
-        <v>22.503328894806923</v>
+        <v>24.500665778961384</v>
       </c>
       <c r="D23" s="3">
-        <v>38.881491344873503</v>
+        <v>41.278295605858858</v>
       </c>
       <c r="E23" s="3">
-        <v>24.101198402130493</v>
+        <v>26.897470039946736</v>
       </c>
       <c r="F23" s="3">
-        <v>43.275632490013315</v>
+        <v>47.270306258322236</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3">
-        <v>33.866666666666667</v>
+      <c r="B24" s="4">
+        <v>36.666666666666664</v>
       </c>
       <c r="C24" s="3">
-        <v>22.63648468708389</v>
+        <v>24.63382157123835</v>
       </c>
       <c r="D24" s="3">
-        <v>39.280958721704394</v>
+        <v>41.67776298268975</v>
       </c>
       <c r="E24" s="3">
-        <v>24.234354194407455</v>
+        <v>27.030625832223702</v>
       </c>
       <c r="F24" s="3">
-        <v>43.675099866844207</v>
+        <v>47.669773635153128</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
-        <v>33.733333333333334</v>
+      <c r="B25" s="4">
+        <v>36.666666666666664</v>
       </c>
       <c r="C25" s="3">
-        <v>22.63648468708389</v>
+        <v>24.766977363515313</v>
       </c>
       <c r="D25" s="3">
-        <v>39.280958721704394</v>
+        <v>41.810918774966709</v>
       </c>
       <c r="E25" s="3">
-        <v>24.367509986684421</v>
+        <v>27.163781624500665</v>
       </c>
       <c r="F25" s="3">
-        <v>43.808255659121173</v>
+        <v>47.802929427430094</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
-        <v>23.6</v>
+      <c r="B26" s="4">
+        <v>24.533333333333335</v>
       </c>
       <c r="C26" s="3">
-        <v>23.96804260985353</v>
+        <v>24.63382157123835</v>
       </c>
       <c r="D26" s="3">
-        <v>24.63382157123835</v>
+        <v>25.29960053262317</v>
       </c>
       <c r="E26" s="3">
-        <v>25.965379494007991</v>
+        <v>26.631158455392811</v>
       </c>
       <c r="F26" s="3">
-        <v>29.161118508655125</v>
+        <v>29.826897470039945</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
-        <v>24.266666666666666</v>
+      <c r="B27" s="4">
+        <v>25.066666666666666</v>
       </c>
       <c r="C27" s="3">
-        <v>24.500665778961384</v>
+        <v>25.166444740346204</v>
       </c>
       <c r="D27" s="3">
-        <v>25.166444740346204</v>
+        <v>25.832223701731024</v>
       </c>
       <c r="E27" s="3">
-        <v>26.498002663115845</v>
+        <v>27.296937416777631</v>
       </c>
       <c r="F27" s="3">
-        <v>29.693741677762983</v>
+        <v>30.492676431424766</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3">
-        <v>23.2</v>
+      <c r="B28" s="4">
+        <v>24.133333333333333</v>
       </c>
       <c r="C28" s="3">
-        <v>23.701731025299601</v>
+        <v>24.367509986684421</v>
       </c>
       <c r="D28" s="3">
-        <v>24.101198402130493</v>
+        <v>24.766977363515313</v>
       </c>
       <c r="E28" s="3">
-        <v>25.699067909454062</v>
+        <v>26.364846870838882</v>
       </c>
       <c r="F28" s="3">
-        <v>28.628495339547271</v>
+        <v>29.294274300932091</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="3">
-        <v>20.8</v>
+      <c r="B29" s="4">
+        <v>21.6</v>
       </c>
       <c r="C29" s="3">
-        <v>21.304926764314249</v>
+        <v>21.837549933422103</v>
       </c>
       <c r="D29" s="3">
-        <v>21.837549933422103</v>
+        <v>22.370173102529961</v>
       </c>
       <c r="E29" s="3">
-        <v>23.169107856191744</v>
+        <v>23.701731025299601</v>
       </c>
       <c r="F29" s="3">
-        <v>25.832223701731024</v>
+        <v>26.364846870838882</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="3">
-        <v>23.866666666666667</v>
+      <c r="B30" s="4">
+        <v>24.8</v>
       </c>
       <c r="C30" s="3">
-        <v>24.234354194407455</v>
+        <v>24.900133155792275</v>
       </c>
       <c r="D30" s="3">
-        <v>24.900133155792275</v>
+        <v>25.565912117177096</v>
       </c>
       <c r="E30" s="3">
-        <v>26.231691078561916</v>
+        <v>26.897470039946736</v>
       </c>
       <c r="F30" s="3">
-        <v>29.427430093209054</v>
+        <v>30.093209054593874</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="3">
-        <v>33.200000000000003</v>
+      <c r="B31" s="4">
+        <v>36.133333333333333</v>
       </c>
       <c r="C31" s="3">
-        <v>21.970705725699069</v>
+        <v>24.101198402130493</v>
       </c>
       <c r="D31" s="3">
-        <v>38.748335552596537</v>
+        <v>41.278295605858858</v>
       </c>
       <c r="E31" s="3">
-        <v>23.701731025299601</v>
+        <v>26.498002663115845</v>
       </c>
       <c r="F31" s="3">
-        <v>43.275632490013315</v>
+        <v>47.403462050599202</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="3">
-        <v>32.266666666666666</v>
+      <c r="B32" s="4">
+        <v>34.93333333333333</v>
       </c>
       <c r="C32" s="3">
-        <v>21.837549933422103</v>
+        <v>23.834886817576564</v>
       </c>
       <c r="D32" s="3">
-        <v>36.884154460719039</v>
+        <v>39.280958721704394</v>
       </c>
       <c r="E32" s="3">
-        <v>23.035952063914781</v>
+        <v>25.699067909454062</v>
       </c>
       <c r="F32" s="3">
-        <v>40.612516644474034</v>
+        <v>44.474034620505989</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="3">
-        <v>32.266666666666666</v>
+      <c r="B33" s="4">
+        <v>34.93333333333333</v>
       </c>
       <c r="C33" s="3">
-        <v>22.237017310252995</v>
+        <v>24.234354194407455</v>
       </c>
       <c r="D33" s="3">
-        <v>36.884154460719039</v>
+        <v>39.280958721704394</v>
       </c>
       <c r="E33" s="3">
-        <v>23.568575233022635</v>
+        <v>26.231691078561916</v>
       </c>
       <c r="F33" s="3">
-        <v>40.213049267643143</v>
+        <v>44.074567243675098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>